<commit_message>
Update Interview zur Anforderungserhebung.xlsx
</commit_message>
<xml_diff>
--- a/Interview zur Anforderungserhebung.xlsx
+++ b/Interview zur Anforderungserhebung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06B37BE-06FC-4759-8F80-EC525BAA6EE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C27F7B-EE79-4573-AEAD-DC52F7103CEB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Fragen</t>
   </si>
@@ -170,6 +170,9 @@
   </si>
   <si>
     <t>EINFÜHRUNG / IMPLEMENTIERUNG / DATENMIGRATION (inkl. Schulung)</t>
+  </si>
+  <si>
+    <t>Spezifischer Teil</t>
   </si>
 </sst>
 </file>
@@ -396,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,9 +407,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -451,6 +451,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -732,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -749,434 +758,438 @@
     <col min="7" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="1" customFormat="1" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="13"/>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:6" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-    </row>
-    <row r="7" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-    </row>
-    <row r="9" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-    </row>
-    <row r="11" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-    </row>
-    <row r="15" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-    </row>
-    <row r="16" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-    </row>
-    <row r="17" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-    </row>
-    <row r="18" spans="1:6" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A18" s="12" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" ht="51" x14ac:dyDescent="0.2">
+      <c r="A31" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
+      <c r="B31" s="12"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="12"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-    </row>
-    <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-    </row>
-    <row r="22" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-    </row>
-    <row r="24" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-    </row>
-    <row r="25" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-    </row>
-    <row r="26" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-    </row>
-    <row r="27" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="8"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-    </row>
-    <row r="28" spans="1:6" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A28" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="8"/>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-    </row>
-    <row r="29" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-    </row>
-    <row r="31" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-    </row>
-    <row r="32" spans="1:6" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:6" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="13"/>
+      <c r="B34" s="12"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A37" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-    </row>
-    <row r="36" spans="1:6" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
-    </row>
-    <row r="37" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
-    </row>
-    <row r="38" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="11"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-      <c r="F39" s="8"/>
-    </row>
-    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16" t="s">
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="10"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
-    </row>
-    <row r="41" spans="1:6" s="1" customFormat="1" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
-    </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="1:6" s="1" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A45" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Revert "Update Interview zur Anforderungserhebung.xlsx"
This reverts commit 15e0fa4f1ecf717279aa5a6cdf3581db655a61b3.
</commit_message>
<xml_diff>
--- a/Interview zur Anforderungserhebung.xlsx
+++ b/Interview zur Anforderungserhebung.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4CFB60-3442-417E-95BE-4A0CD64C689D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AC3D10B-85FA-41E4-AB04-7A92C00DF43D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="465" windowWidth="25605" windowHeight="14475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Derzeitiges CRM-System</t>
   </si>
@@ -226,12 +226,6 @@
   </si>
   <si>
     <t>Existieren Warn- und Erinnerungsfunktionen beim Aussenden von Mails?</t>
-  </si>
-  <si>
-    <t>crm.ie.jku</t>
-  </si>
-  <si>
-    <t>Übersicht --&gt; Kontakte, events, mails</t>
   </si>
 </sst>
 </file>
@@ -824,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -867,7 +861,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>54</v>
       </c>
@@ -877,7 +871,7 @@
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
-    <row r="5" spans="1:6" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>55</v>
       </c>
@@ -891,9 +885,7 @@
       <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>64</v>
-      </c>
+      <c r="B6" s="10"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
@@ -923,9 +915,7 @@
       <c r="A9" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="B9" s="5"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="5"/>
@@ -50288,7 +50278,7 @@
       <c r="E54" s="5"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
         <v>28</v>
       </c>

</xml_diff>